<commit_message>
CV hoja de perfiles
</commit_message>
<xml_diff>
--- a/FALEC/doc/Perfiles-Opciones.xlsx
+++ b/FALEC/doc/Perfiles-Opciones.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3737EBE-FEDC-D24C-BBCA-411E1BE405B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61CE007-50F9-824E-AAD6-5C48AE45CF5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="2400" windowWidth="46340" windowHeight="22100" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
+    <workbookView xWindow="4580" yWindow="2400" windowWidth="46340" windowHeight="22100" activeTab="1" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCIONES" sheetId="1" r:id="rId1"/>
     <sheet name="PERFIL" sheetId="2" r:id="rId2"/>
     <sheet name="USUARIO" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="410">
   <si>
     <t>MENU</t>
   </si>
@@ -1172,9 +1173,6 @@
     <t>COTIZACIÓN - CONSULTA</t>
   </si>
   <si>
-    <t>COMPROBANTE ELECTRÓNICO - ADMINISTRACIÓN</t>
-  </si>
-  <si>
     <t>COMPROBANTE ELECTRÓNICO - CONSULTA</t>
   </si>
   <si>
@@ -1239,6 +1237,27 @@
   </si>
   <si>
     <t>A14</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - FACTURA</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - RETENCIÓN</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - NOTA CREDITO</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - NOTA DÉBITO</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - GUÍA REMISIÓN</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - LIQ COMPRA</t>
+  </si>
+  <si>
+    <t>COMPROBANTE ELECTRÓNICO - RECIBOS</t>
   </si>
 </sst>
 </file>
@@ -1625,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14C5F39-A0E2-CB48-9646-33D3507065BE}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4062,7 +4081,7 @@
         <v>196</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>197</v>
@@ -5034,10 +5053,10 @@
         <v>85</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>392</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1">
@@ -5047,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K87" s="1"/>
       <c r="L87" s="1" t="s">
@@ -6048,10 +6067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733BAF54-BF0A-F947-9343-E8FD086E0740}">
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6289,7 +6308,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -6301,12 +6320,12 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>16</v>
+        <v>169</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -6320,7 +6339,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>7</v>
@@ -6334,7 +6353,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -6348,7 +6367,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -6362,7 +6381,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="B27">
         <v>7</v>
@@ -6376,7 +6395,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -6390,7 +6409,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>22</v>
+        <v>175</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -6404,7 +6423,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
+        <v>176</v>
       </c>
       <c r="B30">
         <v>7</v>
@@ -6418,7 +6437,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="B31">
         <v>7</v>
@@ -6432,7 +6451,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="B32">
         <v>7</v>
@@ -6444,9 +6463,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="B33">
         <v>7</v>
@@ -6458,659 +6477,604 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>180</v>
+      </c>
+      <c r="B35">
+        <v>22</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>181</v>
+      </c>
+      <c r="B36">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>182</v>
+      </c>
+      <c r="B37">
+        <v>22</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>183</v>
+      </c>
+      <c r="B38">
+        <v>22</v>
+      </c>
+      <c r="C38">
         <v>27</v>
       </c>
-      <c r="B34">
-        <v>7</v>
-      </c>
-      <c r="C34">
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>184</v>
+      </c>
+      <c r="B39">
+        <v>22</v>
+      </c>
+      <c r="C39">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>185</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>186</v>
+      </c>
+      <c r="B41">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>187</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>188</v>
+      </c>
+      <c r="B43">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>189</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>190</v>
+      </c>
+      <c r="B46">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>191</v>
+      </c>
+      <c r="B47">
+        <v>23</v>
+      </c>
+      <c r="C47">
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>192</v>
+      </c>
+      <c r="B48">
+        <v>23</v>
+      </c>
+      <c r="C48">
+        <v>35</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>193</v>
+      </c>
+      <c r="B49">
+        <v>23</v>
+      </c>
+      <c r="C49">
+        <v>36</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>194</v>
+      </c>
+      <c r="B50">
+        <v>23</v>
+      </c>
+      <c r="C50">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>195</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>196</v>
+      </c>
+      <c r="B52">
+        <v>23</v>
+      </c>
+      <c r="C52">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>197</v>
+      </c>
+      <c r="B53">
+        <v>23</v>
+      </c>
+      <c r="C53">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>198</v>
+      </c>
+      <c r="B54">
+        <v>23</v>
+      </c>
+      <c r="C54">
+        <v>41</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>199</v>
+      </c>
+      <c r="B55">
+        <v>23</v>
+      </c>
+      <c r="C55">
+        <v>42</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>200</v>
+      </c>
+      <c r="B57">
+        <v>24</v>
+      </c>
+      <c r="C57">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>201</v>
+      </c>
+      <c r="B58">
+        <v>24</v>
+      </c>
+      <c r="C58">
+        <v>43</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>202</v>
+      </c>
+      <c r="B59">
+        <v>24</v>
+      </c>
+      <c r="C59">
+        <v>44</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>203</v>
+      </c>
+      <c r="B60">
+        <v>24</v>
+      </c>
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>204</v>
+      </c>
+      <c r="B61">
+        <v>24</v>
+      </c>
+      <c r="C61">
+        <v>46</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>205</v>
+      </c>
+      <c r="B62">
+        <v>24</v>
+      </c>
+      <c r="C62">
+        <v>47</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>206</v>
+      </c>
+      <c r="B63">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>48</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>207</v>
+      </c>
+      <c r="B64">
+        <v>24</v>
+      </c>
+      <c r="C64">
+        <v>49</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>208</v>
+      </c>
+      <c r="B65">
+        <v>24</v>
+      </c>
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>209</v>
+      </c>
+      <c r="B67">
         <v>25</v>
       </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>28</v>
-      </c>
-      <c r="B35">
-        <v>7</v>
-      </c>
-      <c r="C35">
+      <c r="C67">
+        <v>13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>210</v>
+      </c>
+      <c r="B68">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>51</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>211</v>
+      </c>
+      <c r="B69">
+        <v>25</v>
+      </c>
+      <c r="C69">
+        <v>52</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>212</v>
+      </c>
+      <c r="B70">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>53</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>213</v>
+      </c>
+      <c r="B71">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>54</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>214</v>
+      </c>
+      <c r="B72">
+        <v>25</v>
+      </c>
+      <c r="C72">
+        <v>55</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>215</v>
+      </c>
+      <c r="B73">
+        <v>25</v>
+      </c>
+      <c r="C73">
+        <v>56</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>216</v>
+      </c>
+      <c r="B74">
+        <v>25</v>
+      </c>
+      <c r="C74">
+        <v>57</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>217</v>
+      </c>
+      <c r="B75">
+        <v>25</v>
+      </c>
+      <c r="C75">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>218</v>
+      </c>
+      <c r="B77">
         <v>26</v>
       </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>29</v>
-      </c>
-      <c r="B36">
-        <v>7</v>
-      </c>
-      <c r="C36">
-        <v>27</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>30</v>
-      </c>
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>28</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>31</v>
-      </c>
-      <c r="B38">
-        <v>7</v>
-      </c>
-      <c r="C38">
-        <v>29</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>32</v>
-      </c>
-      <c r="B39">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <v>30</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>33</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-      <c r="C40">
-        <v>31</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>34</v>
-      </c>
-      <c r="B41">
-        <v>7</v>
-      </c>
-      <c r="C41">
-        <v>32</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>35</v>
-      </c>
-      <c r="B42">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>33</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>36</v>
-      </c>
-      <c r="B43">
-        <v>7</v>
-      </c>
-      <c r="C43">
-        <v>34</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>37</v>
-      </c>
-      <c r="B44">
-        <v>7</v>
-      </c>
-      <c r="C44">
-        <v>35</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>38</v>
-      </c>
-      <c r="B45">
-        <v>7</v>
-      </c>
-      <c r="C45">
-        <v>36</v>
-      </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>39</v>
-      </c>
-      <c r="B46">
-        <v>7</v>
-      </c>
-      <c r="C46">
-        <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>40</v>
-      </c>
-      <c r="B47">
-        <v>7</v>
-      </c>
-      <c r="C47">
-        <v>38</v>
-      </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>41</v>
-      </c>
-      <c r="B48">
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <v>39</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>42</v>
-      </c>
-      <c r="B49">
-        <v>7</v>
-      </c>
-      <c r="C49">
-        <v>40</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>43</v>
-      </c>
-      <c r="B50">
-        <v>7</v>
-      </c>
-      <c r="C50">
-        <v>41</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>44</v>
-      </c>
-      <c r="B51">
-        <v>7</v>
-      </c>
-      <c r="C51">
-        <v>42</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>45</v>
-      </c>
-      <c r="B52">
-        <v>7</v>
-      </c>
-      <c r="C52">
-        <v>43</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>46</v>
-      </c>
-      <c r="B53">
-        <v>7</v>
-      </c>
-      <c r="C53">
-        <v>44</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>47</v>
-      </c>
-      <c r="B54">
-        <v>7</v>
-      </c>
-      <c r="C54">
-        <v>45</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>48</v>
-      </c>
-      <c r="B55">
-        <v>7</v>
-      </c>
-      <c r="C55">
-        <v>46</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>49</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="C56">
-        <v>47</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>50</v>
-      </c>
-      <c r="B57">
-        <v>7</v>
-      </c>
-      <c r="C57">
-        <v>48</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>51</v>
-      </c>
-      <c r="B58">
-        <v>7</v>
-      </c>
-      <c r="C58">
-        <v>49</v>
-      </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>52</v>
-      </c>
-      <c r="B59">
-        <v>7</v>
-      </c>
-      <c r="C59">
-        <v>50</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>53</v>
-      </c>
-      <c r="B60">
-        <v>7</v>
-      </c>
-      <c r="C60">
-        <v>51</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>54</v>
-      </c>
-      <c r="B61">
-        <v>7</v>
-      </c>
-      <c r="C61">
-        <v>52</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>55</v>
-      </c>
-      <c r="B62">
-        <v>7</v>
-      </c>
-      <c r="C62">
-        <v>53</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>56</v>
-      </c>
-      <c r="B63">
-        <v>7</v>
-      </c>
-      <c r="C63">
-        <v>54</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>57</v>
-      </c>
-      <c r="B64">
-        <v>7</v>
-      </c>
-      <c r="C64">
-        <v>55</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>58</v>
-      </c>
-      <c r="B65">
-        <v>7</v>
-      </c>
-      <c r="C65">
-        <v>56</v>
-      </c>
-      <c r="D65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="C77">
+        <v>13</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>219</v>
+      </c>
+      <c r="B78">
+        <v>26</v>
+      </c>
+      <c r="C78">
         <v>59</v>
       </c>
-      <c r="B66">
-        <v>7</v>
-      </c>
-      <c r="C66">
-        <v>57</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>220</v>
+      </c>
+      <c r="B79">
+        <v>26</v>
+      </c>
+      <c r="C79">
         <v>60</v>
       </c>
-      <c r="B67">
-        <v>7</v>
-      </c>
-      <c r="C67">
-        <v>58</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>221</v>
+      </c>
+      <c r="B80">
+        <v>26</v>
+      </c>
+      <c r="C80">
         <v>61</v>
-      </c>
-      <c r="B68">
-        <v>7</v>
-      </c>
-      <c r="C68">
-        <v>59</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>62</v>
-      </c>
-      <c r="B69">
-        <v>7</v>
-      </c>
-      <c r="C69">
-        <v>60</v>
-      </c>
-      <c r="D69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>63</v>
-      </c>
-      <c r="B70">
-        <v>7</v>
-      </c>
-      <c r="C70">
-        <v>61</v>
-      </c>
-      <c r="D70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>64</v>
-      </c>
-      <c r="B71">
-        <v>7</v>
-      </c>
-      <c r="C71">
-        <v>62</v>
-      </c>
-      <c r="D71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>65</v>
-      </c>
-      <c r="B72">
-        <v>7</v>
-      </c>
-      <c r="C72">
-        <v>63</v>
-      </c>
-      <c r="D72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>66</v>
-      </c>
-      <c r="B73">
-        <v>7</v>
-      </c>
-      <c r="C73">
-        <v>64</v>
-      </c>
-      <c r="D73" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>67</v>
-      </c>
-      <c r="B74">
-        <v>7</v>
-      </c>
-      <c r="C74">
-        <v>65</v>
-      </c>
-      <c r="D74" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>68</v>
-      </c>
-      <c r="B75">
-        <v>7</v>
-      </c>
-      <c r="C75">
-        <v>66</v>
-      </c>
-      <c r="D75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>69</v>
-      </c>
-      <c r="B76">
-        <v>7</v>
-      </c>
-      <c r="C76">
-        <v>67</v>
-      </c>
-      <c r="D76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>70</v>
-      </c>
-      <c r="B77">
-        <v>7</v>
-      </c>
-      <c r="C77">
-        <v>68</v>
-      </c>
-      <c r="D77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>71</v>
-      </c>
-      <c r="B78">
-        <v>7</v>
-      </c>
-      <c r="C78">
-        <v>69</v>
-      </c>
-      <c r="D78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>72</v>
-      </c>
-      <c r="B79">
-        <v>7</v>
-      </c>
-      <c r="C79">
-        <v>70</v>
-      </c>
-      <c r="D79" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>73</v>
-      </c>
-      <c r="B80">
-        <v>7</v>
-      </c>
-      <c r="C80">
-        <v>71</v>
       </c>
       <c r="D80" t="s">
         <v>6</v>
@@ -7118,13 +7082,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C81">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D81" t="s">
         <v>6</v>
@@ -7132,86 +7096,86 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="B82">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C82">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>224</v>
+      </c>
+      <c r="B83">
+        <v>26</v>
+      </c>
+      <c r="C83">
+        <v>64</v>
+      </c>
+      <c r="D83" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>76</v>
+        <v>225</v>
       </c>
       <c r="B84">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C84">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
-      </c>
-      <c r="E84" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>77</v>
+        <v>226</v>
       </c>
       <c r="B85">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C85">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>78</v>
-      </c>
-      <c r="B86">
-        <v>8</v>
-      </c>
-      <c r="C86">
-        <v>16</v>
-      </c>
-      <c r="D86" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>79</v>
+        <v>227</v>
       </c>
       <c r="B87">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C87">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>80</v>
+        <v>228</v>
       </c>
       <c r="B88">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C88">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -7219,13 +7183,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>81</v>
+        <v>229</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C89">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -7233,13 +7197,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>82</v>
+        <v>230</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C90">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
@@ -7247,13 +7211,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>83</v>
+        <v>231</v>
       </c>
       <c r="B91">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C91">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -7261,69 +7225,44 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>84</v>
+        <v>232</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C92">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="D92" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>85</v>
-      </c>
-      <c r="B93">
-        <v>8</v>
-      </c>
-      <c r="C93">
-        <v>31</v>
-      </c>
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>86</v>
-      </c>
-      <c r="B94">
-        <v>8</v>
-      </c>
-      <c r="C94">
-        <v>32</v>
-      </c>
-      <c r="D94" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B95">
         <v>8</v>
       </c>
       <c r="C95">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
+      </c>
+      <c r="E95" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B96">
         <v>8</v>
       </c>
       <c r="C96">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -7331,13 +7270,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B97">
         <v>8</v>
       </c>
       <c r="C97">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -7345,13 +7284,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B98">
         <v>8</v>
       </c>
       <c r="C98">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -7359,13 +7298,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B99">
         <v>8</v>
       </c>
       <c r="C99">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -7373,13 +7312,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B100">
         <v>8</v>
       </c>
       <c r="C100">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -7387,13 +7326,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B101">
         <v>8</v>
       </c>
       <c r="C101">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
@@ -7401,13 +7340,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B102">
         <v>8</v>
       </c>
       <c r="C102">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
@@ -7415,13 +7354,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B103">
         <v>8</v>
       </c>
       <c r="C103">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
@@ -7429,13 +7368,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B104">
         <v>8</v>
       </c>
       <c r="C104">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
@@ -7443,13 +7382,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B105">
         <v>8</v>
       </c>
       <c r="C105">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -7457,13 +7396,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B106">
         <v>8</v>
       </c>
       <c r="C106">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
@@ -7471,13 +7410,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B107">
         <v>8</v>
       </c>
       <c r="C107">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -7485,13 +7424,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B108">
         <v>8</v>
       </c>
       <c r="C108">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -7499,13 +7438,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B109">
         <v>8</v>
       </c>
       <c r="C109">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -7513,13 +7452,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B110">
         <v>8</v>
       </c>
       <c r="C110">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
@@ -7527,13 +7466,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B111">
         <v>8</v>
       </c>
       <c r="C111">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -7541,271 +7480,282 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B112">
         <v>8</v>
       </c>
       <c r="C112">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B113">
         <v>8</v>
       </c>
       <c r="C113">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D113" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B114">
         <v>8</v>
       </c>
       <c r="C114">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D114" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B115">
         <v>8</v>
       </c>
       <c r="C115">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D115" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B116">
         <v>8</v>
       </c>
       <c r="C116">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D116" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B117">
         <v>8</v>
       </c>
       <c r="C117">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D117" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B118">
         <v>8</v>
       </c>
       <c r="C118">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D118" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>100</v>
+      </c>
+      <c r="B119">
+        <v>8</v>
+      </c>
+      <c r="C119">
+        <v>55</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D120" t="s">
         <v>6</v>
       </c>
-      <c r="E120" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B121">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C121">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B122">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C122">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D122" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B123">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C123">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D123" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B124">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C124">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D124" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B125">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C125">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D125" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B126">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C126">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D126" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B127">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C127">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>109</v>
+      </c>
+      <c r="B128">
+        <v>8</v>
+      </c>
+      <c r="C128">
+        <v>69</v>
+      </c>
+      <c r="D128" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B129">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C129">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D129" t="s">
-        <v>6</v>
-      </c>
-      <c r="E129" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130">
-        <v>120</v>
-      </c>
-      <c r="B130">
-        <v>10</v>
-      </c>
-      <c r="C130">
-        <v>74</v>
-      </c>
-      <c r="D130" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B131">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C131">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="D131" t="s">
         <v>6</v>
+      </c>
+      <c r="E131" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B132">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C132">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D132" t="s">
         <v>6</v>
@@ -7813,13 +7763,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B133">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C133">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D133" t="s">
         <v>6</v>
@@ -7827,13 +7777,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B134">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C134">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D134" t="s">
         <v>6</v>
@@ -7841,44 +7791,55 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B135">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C135">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>116</v>
+      </c>
+      <c r="B136">
+        <v>9</v>
+      </c>
+      <c r="C136">
+        <v>78</v>
+      </c>
+      <c r="D136" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B137">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C137">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D137" t="s">
         <v>6</v>
-      </c>
-      <c r="E137" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B138">
-        <v>11</v>
-      </c>
-      <c r="C138" s="2">
-        <v>82</v>
+        <v>9</v>
+      </c>
+      <c r="C138">
+        <v>80</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
@@ -7886,331 +7847,342 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B140">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C140">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
       </c>
       <c r="E140" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B141">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C141">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>121</v>
+      </c>
+      <c r="B142">
+        <v>10</v>
+      </c>
+      <c r="C142">
+        <v>76</v>
+      </c>
+      <c r="D142" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B143">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
-      </c>
-      <c r="E143" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B144">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C144">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>124</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+      <c r="C145">
+        <v>79</v>
+      </c>
+      <c r="D145" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B146">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
       </c>
-      <c r="E146" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147">
-        <v>133</v>
-      </c>
-      <c r="B147">
-        <v>14</v>
-      </c>
-      <c r="C147">
-        <v>111</v>
-      </c>
-      <c r="D147" t="s">
-        <v>6</v>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>126</v>
+      </c>
+      <c r="B148">
+        <v>11</v>
+      </c>
+      <c r="C148">
+        <v>81</v>
+      </c>
+      <c r="D148" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B149">
-        <v>15</v>
-      </c>
-      <c r="C149">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="C149" s="2">
+        <v>82</v>
       </c>
       <c r="D149" t="s">
         <v>6</v>
-      </c>
-      <c r="E149" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C151">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D151" t="s">
         <v>6</v>
       </c>
       <c r="E151" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B152">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C152">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D152" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153">
-        <v>137</v>
-      </c>
-      <c r="B153">
-        <v>16</v>
-      </c>
-      <c r="C153">
-        <v>88</v>
-      </c>
-      <c r="D153" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B154">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C154">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D154" t="s">
         <v>6</v>
+      </c>
+      <c r="E154" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B155">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C155">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D155" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156">
-        <v>140</v>
-      </c>
-      <c r="B156">
-        <v>16</v>
-      </c>
-      <c r="C156">
-        <v>91</v>
-      </c>
-      <c r="D156" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B157">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C157">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D157" t="s">
         <v>6</v>
+      </c>
+      <c r="E157" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B158">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C158">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="D158" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159">
-        <v>143</v>
-      </c>
-      <c r="B159">
-        <v>16</v>
-      </c>
-      <c r="C159">
-        <v>94</v>
-      </c>
-      <c r="D159" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161">
-        <v>144</v>
-      </c>
-      <c r="B161">
-        <v>17</v>
-      </c>
-      <c r="C161">
-        <v>86</v>
-      </c>
-      <c r="D161" t="s">
-        <v>6</v>
-      </c>
-      <c r="E161" t="s">
-        <v>395</v>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>134</v>
+      </c>
+      <c r="B160">
+        <v>15</v>
+      </c>
+      <c r="C160">
+        <v>85</v>
+      </c>
+      <c r="D160" t="s">
+        <v>6</v>
+      </c>
+      <c r="E160" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B162">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C162">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D162" t="s">
         <v>6</v>
+      </c>
+      <c r="E162" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B163">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C163">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>137</v>
+      </c>
+      <c r="B164">
+        <v>16</v>
+      </c>
+      <c r="C164">
+        <v>88</v>
+      </c>
+      <c r="D164" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B165">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C165">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D165" t="s">
         <v>6</v>
       </c>
-      <c r="E165" t="s">
-        <v>396</v>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>139</v>
+      </c>
+      <c r="B166">
+        <v>16</v>
+      </c>
+      <c r="C166">
+        <v>90</v>
+      </c>
+      <c r="D166" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B167">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C167">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D167" t="s">
         <v>6</v>
-      </c>
-      <c r="E167" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B168">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C168">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D168" t="s">
         <v>6</v>
@@ -8218,13 +8190,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B169">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C169">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D169" t="s">
         <v>6</v>
@@ -8232,13 +8204,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B170">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C170">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D170" t="s">
         <v>6</v>
@@ -8246,30 +8218,30 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B172">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C172">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D172" t="s">
         <v>6</v>
       </c>
       <c r="E172" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B173">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C173">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D173" t="s">
         <v>6</v>
@@ -8277,83 +8249,61 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B174">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C174">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D174" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175">
-        <v>155</v>
-      </c>
-      <c r="B175">
-        <v>20</v>
-      </c>
-      <c r="C175">
-        <v>103</v>
-      </c>
-      <c r="D175" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B176">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C176">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D176" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177">
-        <v>157</v>
-      </c>
-      <c r="B177">
-        <v>20</v>
-      </c>
-      <c r="C177">
-        <v>105</v>
-      </c>
-      <c r="D177" t="s">
-        <v>6</v>
+      <c r="E176" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B178">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C178">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D178" t="s">
         <v>6</v>
+      </c>
+      <c r="E178" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B179">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C179">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D179" t="s">
         <v>6</v>
@@ -8361,13 +8311,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B180">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C180">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D180" t="s">
         <v>6</v>
@@ -8375,61 +8325,58 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B181">
+        <v>19</v>
+      </c>
+      <c r="C181">
+        <v>99</v>
+      </c>
+      <c r="D181" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>152</v>
+      </c>
+      <c r="B183">
         <v>20</v>
       </c>
-      <c r="C181">
-        <v>109</v>
-      </c>
-      <c r="D181" t="s">
-        <v>6</v>
-      </c>
-      <c r="E181" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182">
-        <v>162</v>
-      </c>
-      <c r="B182">
-        <v>20</v>
-      </c>
-      <c r="C182">
-        <v>110</v>
-      </c>
-      <c r="D182" t="s">
-        <v>6</v>
+      <c r="C183">
+        <v>100</v>
+      </c>
+      <c r="D183" t="s">
+        <v>6</v>
+      </c>
+      <c r="E183" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B184">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C184">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
-      </c>
-      <c r="E184" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B185">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C185">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D185" t="s">
         <v>6</v>
@@ -8437,10 +8384,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B186">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C186">
         <v>103</v>
@@ -8451,13 +8398,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B187">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C187">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D187" t="s">
         <v>6</v>
@@ -8465,13 +8412,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B188">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C188">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D188" t="s">
         <v>6</v>
@@ -8479,15 +8426,161 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189">
+        <v>158</v>
+      </c>
+      <c r="B189">
+        <v>20</v>
+      </c>
+      <c r="C189">
+        <v>106</v>
+      </c>
+      <c r="D189" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>159</v>
+      </c>
+      <c r="B190">
+        <v>20</v>
+      </c>
+      <c r="C190">
+        <v>107</v>
+      </c>
+      <c r="D190" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>160</v>
+      </c>
+      <c r="B191">
+        <v>20</v>
+      </c>
+      <c r="C191">
+        <v>108</v>
+      </c>
+      <c r="D191" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>161</v>
+      </c>
+      <c r="B192">
+        <v>20</v>
+      </c>
+      <c r="C192">
+        <v>109</v>
+      </c>
+      <c r="D192" t="s">
+        <v>6</v>
+      </c>
+      <c r="E192" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>162</v>
+      </c>
+      <c r="B193">
+        <v>20</v>
+      </c>
+      <c r="C193">
+        <v>110</v>
+      </c>
+      <c r="D193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>163</v>
+      </c>
+      <c r="B195">
+        <v>21</v>
+      </c>
+      <c r="C195">
+        <v>100</v>
+      </c>
+      <c r="D195" t="s">
+        <v>6</v>
+      </c>
+      <c r="E195" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>164</v>
+      </c>
+      <c r="B196">
+        <v>21</v>
+      </c>
+      <c r="C196">
+        <v>101</v>
+      </c>
+      <c r="D196" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>165</v>
+      </c>
+      <c r="B197">
+        <v>21</v>
+      </c>
+      <c r="C197">
+        <v>103</v>
+      </c>
+      <c r="D197" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>166</v>
+      </c>
+      <c r="B198">
+        <v>21</v>
+      </c>
+      <c r="C198">
+        <v>105</v>
+      </c>
+      <c r="D198" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>167</v>
+      </c>
+      <c r="B199">
+        <v>21</v>
+      </c>
+      <c r="C199">
+        <v>107</v>
+      </c>
+      <c r="D199" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200">
         <v>168</v>
       </c>
-      <c r="B189">
+      <c r="B200">
         <v>21</v>
       </c>
-      <c r="C189">
+      <c r="C200">
         <v>109</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D200" t="s">
         <v>6</v>
       </c>
     </row>
@@ -8512,13 +8605,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>374</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>370</v>
@@ -8532,7 +8625,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -8546,7 +8639,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -8560,7 +8653,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -8574,7 +8667,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -8588,7 +8681,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -8602,7 +8695,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -8616,7 +8709,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -8630,7 +8723,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -8644,7 +8737,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -8658,7 +8751,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -8672,7 +8765,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -8686,7 +8779,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -8700,7 +8793,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -8714,7 +8807,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -8728,7 +8821,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -8742,7 +8835,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -8756,7 +8849,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -8770,7 +8863,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -8784,7 +8877,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -8798,7 +8891,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -8812,7 +8905,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -8826,7 +8919,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -8840,7 +8933,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -8854,7 +8947,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -8868,7 +8961,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -8882,7 +8975,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -8896,7 +8989,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -8910,7 +9003,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -8924,7 +9017,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -8938,7 +9031,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -8952,7 +9045,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -8966,7 +9059,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -8980,7 +9073,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -8994,7 +9087,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -9008,7 +9101,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -9022,7 +9115,7 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -9036,7 +9129,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -9050,7 +9143,7 @@
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -9064,7 +9157,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -9078,7 +9171,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -9092,7 +9185,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -9106,9 +9199,955 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
+        <v>402</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFAC11B-1AD3-184A-8B72-CE4F30A1CD96}">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>168</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>403</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>169</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>170</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>171</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>172</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>173</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>174</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>175</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>176</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>177</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>178</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>179</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>180</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>181</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>182</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>183</v>
+      </c>
+      <c r="B17">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>184</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>185</v>
+      </c>
+      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>186</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>187</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>188</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>189</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>190</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>191</v>
+      </c>
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>192</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>193</v>
+      </c>
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>194</v>
+      </c>
+      <c r="B29">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>195</v>
+      </c>
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>196</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>197</v>
+      </c>
+      <c r="B32">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>198</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>199</v>
+      </c>
+      <c r="B34">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>200</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>201</v>
+      </c>
+      <c r="B37">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>43</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>202</v>
+      </c>
+      <c r="B38">
+        <v>24</v>
+      </c>
+      <c r="C38">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>203</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39">
+        <v>45</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>204</v>
+      </c>
+      <c r="B40">
+        <v>24</v>
+      </c>
+      <c r="C40">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>205</v>
+      </c>
+      <c r="B41">
+        <v>24</v>
+      </c>
+      <c r="C41">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>206</v>
+      </c>
+      <c r="B42">
+        <v>24</v>
+      </c>
+      <c r="C42">
+        <v>48</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>207</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>49</v>
+      </c>
       <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>208</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>209</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>210</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>51</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>211</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>52</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>212</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>53</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>213</v>
+      </c>
+      <c r="B50">
+        <v>25</v>
+      </c>
+      <c r="C50">
+        <v>54</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>214</v>
+      </c>
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51">
+        <v>55</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>215</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>56</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>216</v>
+      </c>
+      <c r="B53">
+        <v>25</v>
+      </c>
+      <c r="C53">
+        <v>57</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>217</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>218</v>
+      </c>
+      <c r="B56">
+        <v>26</v>
+      </c>
+      <c r="C56">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>219</v>
+      </c>
+      <c r="B57">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>59</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>220</v>
+      </c>
+      <c r="B58">
+        <v>26</v>
+      </c>
+      <c r="C58">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>221</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>61</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>222</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>223</v>
+      </c>
+      <c r="B61">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>224</v>
+      </c>
+      <c r="B62">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>225</v>
+      </c>
+      <c r="B63">
+        <v>26</v>
+      </c>
+      <c r="C63">
+        <v>65</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>226</v>
+      </c>
+      <c r="B64">
+        <v>26</v>
+      </c>
+      <c r="C64">
+        <v>66</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>227</v>
+      </c>
+      <c r="B66">
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>228</v>
+      </c>
+      <c r="B67">
+        <v>27</v>
+      </c>
+      <c r="C67">
+        <v>67</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>229</v>
+      </c>
+      <c r="B68">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>68</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>230</v>
+      </c>
+      <c r="B69">
+        <v>27</v>
+      </c>
+      <c r="C69">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>231</v>
+      </c>
+      <c r="B70">
+        <v>27</v>
+      </c>
+      <c r="C70">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>232</v>
+      </c>
+      <c r="B71">
+        <v>27</v>
+      </c>
+      <c r="C71">
+        <v>71</v>
+      </c>
+      <c r="D71" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CV pantalla de perfiles selección de perfiles
</commit_message>
<xml_diff>
--- a/FALEC/doc/Perfiles-Opciones.xlsx
+++ b/FALEC/doc/Perfiles-Opciones.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61CE007-50F9-824E-AAD6-5C48AE45CF5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F026E-9D25-DC4B-95CB-479DC8D344FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="2400" windowWidth="46340" windowHeight="22100" activeTab="1" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
+    <workbookView xWindow="4580" yWindow="2400" windowWidth="46340" windowHeight="22100" activeTab="4" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCIONES" sheetId="1" r:id="rId1"/>
     <sheet name="PERFIL" sheetId="2" r:id="rId2"/>
     <sheet name="USUARIO" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="PER PREDEFINIDOS" sheetId="4" r:id="rId4"/>
+    <sheet name="PER PRED ACCESO" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="426">
   <si>
     <t>MENU</t>
   </si>
@@ -1258,6 +1259,54 @@
   </si>
   <si>
     <t>COMPROBANTE ELECTRÓNICO - RECIBOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador </t>
+  </si>
+  <si>
+    <t>Administra toda la cuenta del negocio en el sistema</t>
+  </si>
+  <si>
+    <t>fa-gears</t>
+  </si>
+  <si>
+    <t>Gerencia</t>
+  </si>
+  <si>
+    <t>Acceso a todas las opcines, excepto a la configuración de la cuenta.</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Acceso al punto de venta, inventarios</t>
+  </si>
+  <si>
+    <t>Acceso a facturación, clientes, consulta de comprobantes</t>
+  </si>
+  <si>
+    <t>Bodega</t>
+  </si>
+  <si>
+    <t>Acceso a Inventarios, Guías de remisión</t>
+  </si>
+  <si>
+    <t>Contabilidad</t>
+  </si>
+  <si>
+    <t>Acceso Comprobantes, emitidos, comprobantes recibidos SRI, Compras, Gastos, cuentas por cobrar, caja chica y reportes</t>
+  </si>
+  <si>
+    <t>Sólo Lectura</t>
+  </si>
+  <si>
+    <t>Acceso de lectura al sistema, excepto la configuración de la cuenta del negocio.</t>
+  </si>
+  <si>
+    <t>idsegperfilpredefinido</t>
+  </si>
+  <si>
+    <t>idsegperfildefinidoperfil</t>
   </si>
 </sst>
 </file>
@@ -6069,8 +6118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733BAF54-BF0A-F947-9343-E8FD086E0740}">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="B195" activeCellId="5" sqref="B2 B95 B160 B172 B178 B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9212,942 +9261,1378 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFAC11B-1AD3-184A-8B72-CE4F30A1CD96}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD71"/>
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>168</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="C1">
-        <v>13</v>
+      <c r="B8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C8" t="s">
+        <v>423</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF436373-8ED8-4B48-8CCA-55BF41142A1A}">
+  <dimension ref="A1:G87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" t="s">
+        <v>424</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>410</v>
+      </c>
+      <c r="G2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>170</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>171</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>172</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>173</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>174</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>175</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>176</v>
-      </c>
-      <c r="B9">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>413</v>
+      </c>
+      <c r="G25" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>177</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>178</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>179</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>180</v>
-      </c>
-      <c r="B14">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>181</v>
-      </c>
-      <c r="B15">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>182</v>
-      </c>
-      <c r="B16">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>183</v>
-      </c>
-      <c r="B17">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>184</v>
-      </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>185</v>
-      </c>
-      <c r="B19">
-        <v>22</v>
-      </c>
-      <c r="C19">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>186</v>
-      </c>
-      <c r="B20">
-        <v>22</v>
-      </c>
-      <c r="C20">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>187</v>
-      </c>
-      <c r="B21">
-        <v>22</v>
-      </c>
-      <c r="C21">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>188</v>
-      </c>
-      <c r="B22">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>189</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>190</v>
-      </c>
-      <c r="B25">
-        <v>23</v>
-      </c>
-      <c r="C25">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>191</v>
-      </c>
-      <c r="B26">
-        <v>23</v>
-      </c>
-      <c r="C26">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>192</v>
-      </c>
-      <c r="B27">
-        <v>23</v>
-      </c>
-      <c r="C27">
-        <v>35</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>193</v>
-      </c>
-      <c r="B28">
-        <v>23</v>
-      </c>
-      <c r="C28">
-        <v>36</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>194</v>
-      </c>
-      <c r="B29">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>37</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>195</v>
-      </c>
-      <c r="B30">
-        <v>23</v>
-      </c>
-      <c r="C30">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>196</v>
-      </c>
-      <c r="B31">
-        <v>23</v>
-      </c>
-      <c r="C31">
-        <v>39</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>197</v>
       </c>
       <c r="B32">
         <v>23</v>
       </c>
       <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>26</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>27</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>198</v>
-      </c>
-      <c r="B33">
-        <v>23</v>
-      </c>
-      <c r="C33">
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>41</v>
       </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>199</v>
-      </c>
-      <c r="B34">
-        <v>23</v>
-      </c>
-      <c r="C34">
+      <c r="B43">
+        <v>18</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>200</v>
-      </c>
-      <c r="B36">
-        <v>24</v>
-      </c>
-      <c r="C36">
+      <c r="B44">
+        <v>19</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>415</v>
+      </c>
+      <c r="G47" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>307</v>
+      </c>
+      <c r="G53" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>17</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>19</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>60</v>
+      </c>
+      <c r="B65">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>418</v>
+      </c>
+      <c r="G65" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>61</v>
+      </c>
+      <c r="B66">
+        <v>17</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>62</v>
+      </c>
+      <c r="B67">
+        <v>19</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>63</v>
+      </c>
+      <c r="B68">
+        <v>20</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>64</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" t="s">
+        <v>420</v>
+      </c>
+      <c r="G70" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>65</v>
+      </c>
+      <c r="B71">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>66</v>
+      </c>
+      <c r="B72">
+        <v>9</v>
+      </c>
+      <c r="C72">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>67</v>
+      </c>
+      <c r="B73">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>68</v>
+      </c>
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>69</v>
+      </c>
+      <c r="B75">
         <v>13</v>
       </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>201</v>
-      </c>
-      <c r="B37">
-        <v>24</v>
-      </c>
-      <c r="C37">
-        <v>43</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>202</v>
-      </c>
-      <c r="B38">
-        <v>24</v>
-      </c>
-      <c r="C38">
-        <v>44</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>203</v>
-      </c>
-      <c r="B39">
-        <v>24</v>
-      </c>
-      <c r="C39">
-        <v>45</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>204</v>
-      </c>
-      <c r="B40">
-        <v>24</v>
-      </c>
-      <c r="C40">
-        <v>46</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>205</v>
-      </c>
-      <c r="B41">
-        <v>24</v>
-      </c>
-      <c r="C41">
-        <v>47</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>206</v>
-      </c>
-      <c r="B42">
-        <v>24</v>
-      </c>
-      <c r="C42">
-        <v>48</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>207</v>
-      </c>
-      <c r="B43">
-        <v>24</v>
-      </c>
-      <c r="C43">
-        <v>49</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>208</v>
-      </c>
-      <c r="B44">
-        <v>24</v>
-      </c>
-      <c r="C44">
-        <v>50</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>209</v>
-      </c>
-      <c r="B46">
-        <v>25</v>
-      </c>
-      <c r="C46">
-        <v>13</v>
-      </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>210</v>
-      </c>
-      <c r="B47">
-        <v>25</v>
-      </c>
-      <c r="C47">
-        <v>51</v>
-      </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>211</v>
-      </c>
-      <c r="B48">
-        <v>25</v>
-      </c>
-      <c r="C48">
-        <v>52</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>212</v>
-      </c>
-      <c r="B49">
-        <v>25</v>
-      </c>
-      <c r="C49">
-        <v>53</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>213</v>
-      </c>
-      <c r="B50">
-        <v>25</v>
-      </c>
-      <c r="C50">
-        <v>54</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>214</v>
-      </c>
-      <c r="B51">
-        <v>25</v>
-      </c>
-      <c r="C51">
-        <v>55</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>215</v>
-      </c>
-      <c r="B52">
-        <v>25</v>
-      </c>
-      <c r="C52">
-        <v>56</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>216</v>
-      </c>
-      <c r="B53">
-        <v>25</v>
-      </c>
-      <c r="C53">
-        <v>57</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>217</v>
-      </c>
-      <c r="B54">
-        <v>25</v>
-      </c>
-      <c r="C54">
-        <v>58</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>218</v>
-      </c>
-      <c r="B56">
-        <v>26</v>
-      </c>
-      <c r="C56">
-        <v>13</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>219</v>
-      </c>
-      <c r="B57">
-        <v>26</v>
-      </c>
-      <c r="C57">
-        <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>220</v>
-      </c>
-      <c r="B58">
-        <v>26</v>
-      </c>
-      <c r="C58">
-        <v>60</v>
-      </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>221</v>
-      </c>
-      <c r="B59">
-        <v>26</v>
-      </c>
-      <c r="C59">
-        <v>61</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>222</v>
-      </c>
-      <c r="B60">
-        <v>26</v>
-      </c>
-      <c r="C60">
-        <v>62</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>223</v>
-      </c>
-      <c r="B61">
-        <v>26</v>
-      </c>
-      <c r="C61">
-        <v>63</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>224</v>
-      </c>
-      <c r="B62">
-        <v>26</v>
-      </c>
-      <c r="C62">
-        <v>64</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>225</v>
-      </c>
-      <c r="B63">
-        <v>26</v>
-      </c>
-      <c r="C63">
-        <v>65</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>226</v>
-      </c>
-      <c r="B64">
-        <v>26</v>
-      </c>
-      <c r="C64">
-        <v>66</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>227</v>
-      </c>
-      <c r="B66">
-        <v>27</v>
-      </c>
-      <c r="C66">
-        <v>13</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>228</v>
-      </c>
-      <c r="B67">
-        <v>27</v>
-      </c>
-      <c r="C67">
-        <v>67</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>229</v>
-      </c>
-      <c r="B68">
-        <v>27</v>
-      </c>
-      <c r="C68">
-        <v>68</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>230</v>
-      </c>
-      <c r="B69">
-        <v>27</v>
-      </c>
-      <c r="C69">
-        <v>69</v>
-      </c>
-      <c r="D69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>231</v>
-      </c>
-      <c r="B70">
-        <v>27</v>
-      </c>
-      <c r="C70">
+      <c r="C75">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
         <v>70</v>
       </c>
-      <c r="D70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>232</v>
-      </c>
-      <c r="B71">
-        <v>27</v>
-      </c>
-      <c r="C71">
+      <c r="B76">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
         <v>71</v>
       </c>
-      <c r="D71" t="s">
+      <c r="B77">
+        <v>17</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>72</v>
+      </c>
+      <c r="B78">
+        <v>18</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>73</v>
+      </c>
+      <c r="B79">
+        <v>19</v>
+      </c>
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>74</v>
+      </c>
+      <c r="B80">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>75</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" t="s">
+        <v>422</v>
+      </c>
+      <c r="G82" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>76</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>77</v>
+      </c>
+      <c r="B84">
+        <v>15</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>78</v>
+      </c>
+      <c r="B85">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>79</v>
+      </c>
+      <c r="B86">
+        <v>19</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87">
+        <v>21</v>
+      </c>
+      <c r="C87">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CV calculo de cuentas por cobrar
</commit_message>
<xml_diff>
--- a/FALEC/doc/Perfiles-Opciones.xlsx
+++ b/FALEC/doc/Perfiles-Opciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F026E-9D25-DC4B-95CB-479DC8D344FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502DFB6-20FB-E141-B101-EF8DBA47C354}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="2400" windowWidth="46340" windowHeight="22100" activeTab="4" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
+    <workbookView xWindow="13020" yWindow="2780" windowWidth="46340" windowHeight="22100" activeTab="2" xr2:uid="{01D14F21-1573-B741-8681-0D009D3261FD}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCIONES" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="426">
   <si>
     <t>MENU</t>
   </si>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14C5F39-A0E2-CB48-9646-33D3507065BE}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+    <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6118,8 +6118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733BAF54-BF0A-F947-9343-E8FD086E0740}">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B195" activeCellId="5" sqref="B2 B95 B160 B172 B178 B195"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8642,7 +8642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F780CAAF-0622-F04A-A32D-F8A6512B7E68}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9444,10 +9444,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF436373-8ED8-4B48-8CCA-55BF41142A1A}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10636,6 +10636,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>81</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>